<commit_message>
Complete the Login test suite
</commit_message>
<xml_diff>
--- a/source/Results/result.xlsx
+++ b/source/Results/result.xlsx
@@ -1,104 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\SM-SeleniumWithPython\source\Results\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
-  <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Xpath</t>
-  </si>
-  <si>
-    <t>Ouput</t>
-  </si>
-  <si>
-    <t>Results</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>admin-123</t>
-  </si>
-  <si>
-    <t>//span[@id="UserNameRequired"]</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>//span[@id="PasswordRequired"]</t>
-  </si>
-  <si>
-    <t>abcd</t>
-  </si>
-  <si>
-    <t>//div[@class='text-danger']</t>
-  </si>
-  <si>
-    <t>Your login attempt was not successful. Please try again.</t>
-  </si>
-  <si>
-    <t>asd-1245</t>
-  </si>
-  <si>
-    <t>//span[@id="Header_LoginViewHeader_LoginName1"]</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="0"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -117,20 +60,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -172,14 +115,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -445,137 +448,211 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="45.77734375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="45.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" style="3" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="3"/>
+    <col width="12.77734375" customWidth="1" style="3" min="1" max="1"/>
+    <col width="11.77734375" customWidth="1" style="3" min="2" max="2"/>
+    <col width="45.77734375" customWidth="1" style="3" min="3" max="3"/>
+    <col width="45.6640625" customWidth="1" style="3" min="4" max="4"/>
+    <col width="12.109375" customWidth="1" style="3" min="5" max="5"/>
+    <col width="8.88671875" customWidth="1" style="3" min="6" max="8"/>
+    <col width="8.88671875" customWidth="1" style="3" min="9" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>4</v>
+    <row r="1" customFormat="1" s="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>UserName</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>Password</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>Xpath</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>Ouput</t>
+        </is>
+      </c>
+      <c r="E1" s="5" t="inlineStr">
+        <is>
+          <t>Results</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="4"/>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>admin-123</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>//span[@id="UserNameRequired"]</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="4"/>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>//span[@id="PasswordRequired"]</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="E3" s="4" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="4"/>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>abcd</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>admin-123</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>//div[@class='text-danger']</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>Your login attempt was not successful. Please try again.</t>
+        </is>
+      </c>
+      <c r="E4" s="4" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="4"/>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>asd-1245</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>//div[@class='text-danger']</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>Your login attempt was not successful. Please try again.</t>
+        </is>
+      </c>
+      <c r="E5" s="4" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="4"/>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>admin-123</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>//span[@id="Header_LoginViewHeader_LoginName1"]</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="E6" s="4" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E6">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="NOT TESTED">
+    <cfRule type="containsText" priority="1" operator="containsText" dxfId="3" text="NOT TESTED">
       <formula>NOT(ISERROR(SEARCH(("NOT TESTED"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="BLOCKED">
+    <cfRule type="containsText" priority="2" operator="containsText" dxfId="2" text="BLOCKED">
       <formula>NOT(ISERROR(SEARCH(("BLOCKED"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="FAIL">
+    <cfRule type="containsText" priority="3" operator="containsText" dxfId="1" text="FAIL">
       <formula>NOT(ISERROR(SEARCH(("FAIL"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" priority="4" operator="containsText" dxfId="0" text="PASS">
       <formula>NOT(ISERROR(SEARCH(("PASS"),(E2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6">
+    <dataValidation sqref="E2:E6" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"PASS,FAIL,Blocked,Not Tested"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>